<commit_message>
finished answers to PS2-1 and PS2-2
</commit_message>
<xml_diff>
--- a/Braden_PS2-1_2.xlsx
+++ b/Braden_PS2-1_2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>PS2-1:</t>
   </si>
@@ -89,43 +89,16 @@
     <t>I</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>V</t>
+    <t>J</t>
+  </si>
+  <si>
+    <t>J isn't a real amino acid, but can be a symbol for ambiguity between I and L. However, J is not in BLOSUM, so I assume these aren't really meant to be genuine amino acid symbols?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -163,11 +136,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -178,6 +154,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -445,11 +424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,17 +437,17 @@
     <col min="2" max="24" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -551,7 +530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -589,7 +568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -600,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -608,224 +587,220 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="H14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H16" t="s">
         <v>16</v>
       </c>
-      <c r="K14" t="s">
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" t="s">
         <v>1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="K16" t="s">
         <v>18</v>
       </c>
-      <c r="M14" t="s">
+      <c r="L16" t="s">
         <v>19</v>
       </c>
-      <c r="N14" t="s">
-        <v>23</v>
-      </c>
-      <c r="O14" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>17</v>
-      </c>
-      <c r="R14" t="s">
-        <v>26</v>
-      </c>
-      <c r="S14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T14" t="s">
-        <v>4</v>
-      </c>
-      <c r="U14" t="s">
-        <v>28</v>
-      </c>
-      <c r="V14" t="s">
-        <v>29</v>
-      </c>
-      <c r="W14" t="s">
-        <v>30</v>
-      </c>
-      <c r="X14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
+      <c r="M16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18">
-        <v>9</v>
-      </c>
-      <c r="M18">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>5</v>
       </c>
+      <c r="J19">
+        <v>7</v>
+      </c>
       <c r="K19">
-        <v>7</v>
-      </c>
-      <c r="L19">
         <v>2</v>
+      </c>
+      <c r="M19">
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="J20">
+        <v>16</v>
+      </c>
+      <c r="K20">
+        <v>9</v>
+      </c>
+      <c r="L20">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="M21">
+      <c r="J21">
+        <v>16</v>
+      </c>
+      <c r="L21">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>7</v>
-      </c>
-      <c r="H22">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="L22">
+        <v>9</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
       </c>
       <c r="G23">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>11</v>
-      </c>
-      <c r="J24">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="G25">
+        <v>11</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="3:3" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="3:13" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C13:M15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>